<commit_message>
Add reconnect method, add state control..
</commit_message>
<xml_diff>
--- a/xiaomi_data_analysis.xlsx
+++ b/xiaomi_data_analysis.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="小米手环service列表" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -15,8 +15,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="C48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Key Value
+0 No Alert
+1 Mild Alert
+2 High Alert
+3 - 255 Reserved</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="169">
   <si>
     <t>handle range</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -645,10 +683,6 @@
   </si>
   <si>
     <t>write 27 ff05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>write 47 ff0e</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -685,12 +719,25 @@
 04--&gt; 未充电的状态 02 充电ing 03 充满</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>1802
+(immediate alert)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>write 20 ff02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>write 47 ff0d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -714,6 +761,19 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -723,7 +783,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -731,16 +791,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1043,42 +1124,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.75" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.375" customWidth="1"/>
     <col min="9" max="9" width="66" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -1086,30 +1167,34 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A2" s="1">
+      <c r="A2" s="6">
         <v>1800</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -1120,13 +1205,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C4" s="1" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1137,71 +1225,92 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C5" s="1" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
       <c r="H6" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A7" s="1">
+      <c r="A7" s="6">
         <v>1801</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C8" s="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6">
         <v>2902</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="F8" s="6"/>
       <c r="H8" t="s">
         <v>148</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
       <c r="H9" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1209,13 +1318,16 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C11" s="1" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="6" t="s">
         <v>37</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1223,32 +1335,42 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C12" s="1" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C13" s="1" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="6" t="s">
         <v>72</v>
       </c>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C14" s="1" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="6" t="s">
         <v>39</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -1259,13 +1381,16 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C15" s="1" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="7"/>
+      <c r="E15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="6" t="s">
         <v>40</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -1273,60 +1398,77 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C16" s="1" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="D16" s="7"/>
+      <c r="E16" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C17" s="1" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="D17" s="7"/>
+      <c r="E17" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="F17" s="6"/>
       <c r="H17" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="3:9" ht="148.5" x14ac:dyDescent="0.15">
-      <c r="C18" s="1" t="s">
+    <row r="18" spans="1:9" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="D18" s="7"/>
+      <c r="E18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="6" t="s">
         <v>46</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C19" s="1" t="s">
+      <c r="I18" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C20" s="1" t="s">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="6" t="s">
         <v>48</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -1336,47 +1478,60 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C21" s="1" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C22" s="1" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="6" t="s">
         <v>76</v>
       </c>
+      <c r="F22" s="6"/>
       <c r="H22" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C23" s="1" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C24" s="1" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="D24" s="7"/>
+      <c r="E24" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="6" t="s">
         <v>56</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -1386,47 +1541,60 @@
         <v>126</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C25" s="1" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C26" s="1" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="6" t="s">
         <v>77</v>
       </c>
+      <c r="F26" s="6"/>
       <c r="H26" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C27" s="1" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C28" s="1" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="D28" s="7"/>
+      <c r="E28" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="6" t="s">
         <v>65</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -1436,22 +1604,29 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C29" s="1" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C30" s="1" t="s">
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="D30" s="7"/>
+      <c r="E30" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="6" t="s">
         <v>68</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -1461,24 +1636,31 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C31" s="1" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="D31" s="7"/>
+      <c r="E31" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.15">
-      <c r="C32" s="1" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="D32" s="7"/>
+      <c r="E32" s="6" t="s">
         <v>79</v>
       </c>
+      <c r="F32" s="6"/>
       <c r="H32" s="1" t="s">
         <v>159</v>
       </c>
@@ -1486,23 +1668,31 @@
         <v>130</v>
       </c>
     </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+    </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="6" t="s">
         <v>89</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -1513,30 +1703,34 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C35" s="1" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C36" s="1" t="s">
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" s="6" t="s">
         <v>97</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -1544,30 +1738,34 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C37" s="1" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="6" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C38" s="1" t="s">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" s="6" t="s">
         <v>104</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -1578,30 +1776,34 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C39" s="1" t="s">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" s="6" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C40" s="1" t="s">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="6" t="s">
         <v>110</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -1611,96 +1813,126 @@
         <v>133</v>
       </c>
     </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+    </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
       <c r="H42" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="6" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C44" s="1" t="s">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="6" t="s">
         <v>116</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C45" s="1" t="s">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="D45" s="7"/>
+      <c r="E45" s="6" t="s">
         <v>119</v>
       </c>
+      <c r="F45" s="6"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C46" s="1" t="s">
+      <c r="A46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" s="6" t="s">
         <v>118</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A48" s="1">
-        <v>1802</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A47" s="6"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" ht="27" x14ac:dyDescent="0.15">
+      <c r="A48" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="6" t="s">
         <v>124</v>
       </c>
       <c r="H48" s="1" t="s">
@@ -1712,7 +1944,7 @@
     </row>
     <row r="50" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H50" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="8:9" x14ac:dyDescent="0.15">
@@ -1720,12 +1952,12 @@
         <v>159</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H54" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="8:9" x14ac:dyDescent="0.15">
@@ -1743,7 +1975,7 @@
     </row>
     <row r="60" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H60" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" spans="8:9" x14ac:dyDescent="0.15">
@@ -1788,7 +2020,7 @@
         <v>144</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="8:9" x14ac:dyDescent="0.15">
@@ -1803,6 +2035,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
enable notification: 1. mBluetoothGatt.setCharacteristicNotification(characteristic, enabled); 2.descriptor.setValue 3. mBluetoothGatt.writeDescriptor; The three steps can not be missed.
</commit_message>
<xml_diff>
--- a/xiaomi_data_analysis.xlsx
+++ b/xiaomi_data_analysis.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="172">
   <si>
     <t>handle range</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -730,6 +730,20 @@
   </si>
   <si>
     <t>write 47 ff0d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ff06(Handle Value Notification
+): 步数值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2c 00 00 00
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>=44步</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -810,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -822,6 +836,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1127,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1942,12 +1959,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H50" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H52" s="1" t="s">
         <v>159</v>
       </c>
@@ -1955,17 +1972,28 @@
         <v>163</v>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A53" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H54" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H56" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H58" s="1" t="s">
         <v>159</v>
       </c>
@@ -1973,12 +2001,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H60" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H62" s="1" t="s">
         <v>159</v>
       </c>
@@ -1986,7 +2014,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H64" t="s">
         <v>146</v>
       </c>

</xml_diff>